<commit_message>
Updated data set for Board Master
</commit_message>
<xml_diff>
--- a/SqlQueries/DataInsertUpdateQueries/Sprint 3/Boards.xlsx
+++ b/SqlQueries/DataInsertUpdateQueries/Sprint 3/Boards.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="236">
   <si>
     <t>CountryId</t>
   </si>
@@ -721,6 +721,9 @@
   </si>
   <si>
     <t>FAAEM</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1134,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1171,7 +1174,7 @@
         <v>200</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C21" si="0">CONCATENATE("INSERT INTO [dbo].[BoardMaster] ([Board], [Description],[Active],[AddedBy],[AddedDate]) VALUES ('",A3,"','",B3,"',1,1,GETDATE())")</f>
+        <f t="shared" ref="C3:C22" si="0">CONCATENATE("INSERT INTO [dbo].[BoardMaster] ([Board], [Description],[Active],[AddedBy],[AddedDate]) VALUES ('",A3,"','",B3,"',1,1,GETDATE())")</f>
         <v>INSERT INTO [dbo].[BoardMaster] ([Board], [Description],[Active],[AddedBy],[AddedDate]) VALUES ('FAAFP','Fellow of the American Academy of Family Physicians',1,1,GETDATE())</v>
       </c>
     </row>
@@ -1211,7 +1214,7 @@
         <v>INSERT INTO [dbo].[BoardMaster] ([Board], [Description],[Active],[AddedBy],[AddedDate]) VALUES ('FRCPSC','Fellow of the Royal College of Physicians and Surgeons of Canada',1,1,GETDATE())</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5">
+    <row r="7" spans="1:3" ht="31.5">
       <c r="A7" s="6" t="s">
         <v>207</v>
       </c>
@@ -1391,8 +1394,17 @@
         <v>INSERT INTO [dbo].[BoardMaster] ([Board], [Description],[Active],[AddedBy],[AddedDate]) VALUES ('ThD','Doctor of Theology',1,1,GETDATE())</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75">
-      <c r="B22" s="1"/>
+    <row r="22" spans="1:3" ht="16.5">
+      <c r="A22" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [dbo].[BoardMaster] ([Board], [Description],[Active],[AddedBy],[AddedDate]) VALUES ('Other','Other',1,1,GETDATE())</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="15.75">
       <c r="B23" s="1"/>

</xml_diff>